<commit_message>
updated msg constructor and portfolio
</commit_message>
<xml_diff>
--- a/My_Portfolio.xlsx
+++ b/My_Portfolio.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Documents/EECS/TAP/TAP Project/Tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Documents/EECS/TAP/TAP_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{823A08F7-DF79-6444-8AE9-6DD2E020BCEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20F1E5B-9FF4-1F49-A322-778D56BD7AD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{077D8766-08C2-C04D-B333-C950B8A9899D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ticker</t>
   </si>
@@ -56,26 +56,50 @@
     <t>AAPL</t>
   </si>
   <si>
-    <t>ENPH</t>
-  </si>
-  <si>
-    <t>CD</t>
-  </si>
-  <si>
-    <t>ZM</t>
+    <t>FNCL</t>
+  </si>
+  <si>
+    <t>SMH</t>
+  </si>
+  <si>
+    <t>ICLN</t>
+  </si>
+  <si>
+    <t>ACES</t>
+  </si>
+  <si>
+    <t>ARKW</t>
+  </si>
+  <si>
+    <t>TSM</t>
+  </si>
+  <si>
+    <t>NOVA</t>
+  </si>
+  <si>
+    <t>GXTG</t>
+  </si>
+  <si>
+    <t>FANG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,9 +122,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,13 +441,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80592F4-B620-5444-8C00-D0DAB462B072}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -444,83 +473,147 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>210.15</v>
-      </c>
-      <c r="C2" s="1">
-        <v>43983</v>
-      </c>
-      <c r="D2">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="B6" s="1">
+        <v>74.95</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44383</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="F6" s="3">
         <v>0.1</v>
       </c>
-      <c r="F2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>287.10000000000002</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44000</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>0.8</v>
-      </c>
-      <c r="F3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>35.119999999999997</v>
-      </c>
-      <c r="C4" s="1">
-        <v>43983</v>
-      </c>
-      <c r="D4">
-        <v>20</v>
-      </c>
-      <c r="E4">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1">
+        <v>150.9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>44383</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
+        <v>91.65</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44383</v>
+      </c>
+      <c r="D11" s="1">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3">
         <v>0.15</v>
       </c>
-      <c r="F4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>300.13</v>
-      </c>
-      <c r="C5" s="1">
-        <v>44000</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>0.2</v>
-      </c>
-      <c r="F5">
-        <v>0.5</v>
+      <c r="F11" s="3">
+        <v>0.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reformatted email and prepared for technical analysis
</commit_message>
<xml_diff>
--- a/My_Portfolio.xlsx
+++ b/My_Portfolio.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tony/Documents/EECS/TAP/TAP_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC91712-5F21-0A42-B893-AA9F94A7BE2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41705669-4F3A-8943-B3FB-DA358A05E5A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2140" windowWidth="28040" windowHeight="17440" xr2:uid="{077D8766-08C2-C04D-B333-C950B8A9899D}"/>
   </bookViews>
@@ -449,7 +449,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,13 +513,21 @@
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="B4" s="1">
+        <v>255.6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>44384</v>
+      </c>
       <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -537,21 +545,13 @@
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1">
-        <v>74.95</v>
-      </c>
-      <c r="C6" s="2">
-        <v>44383</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="1">
-        <v>6</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -564,7 +564,7 @@
         <v>44383</v>
       </c>
       <c r="D7" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7" s="3">
         <v>0.1</v>
@@ -601,33 +601,33 @@
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="1">
+        <v>51.25</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44384</v>
+      </c>
       <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="1">
-        <v>91.65</v>
-      </c>
-      <c r="C11" s="2">
-        <v>44383</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="1">
-        <v>5</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.08</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -640,7 +640,7 @@
         <v>44364</v>
       </c>
       <c r="D12" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E12" s="5">
         <v>0.15</v>

</xml_diff>